<commit_message>
First commit after changes
</commit_message>
<xml_diff>
--- a/DataFiles/Payloads.xlsx
+++ b/DataFiles/Payloads.xlsx
@@ -26,7 +26,7 @@
     <sheet name="BSQL" sheetId="12" r:id="rId12"/>
     <sheet name="HTML" sheetId="13" r:id="rId13"/>
     <sheet name="LDAP" sheetId="14" r:id="rId14"/>
-    <sheet name="TEST" sheetId="15" r:id="rId15"/>
+    <sheet name="HHA" sheetId="15" r:id="rId15"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="649">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="650">
   <si>
     <t>&lt;pre&gt;&lt;!--#exec cmd="/bi*/ca? /et*/passw?" --&gt;&lt;/pre&gt;'</t>
   </si>
@@ -1986,7 +1986,10 @@
     <t>{{[] .__ Class __.__ base __.__ subclasses __ ()}}</t>
   </si>
   <si>
-    <t>id;</t>
+    <t>HOST Header Attack</t>
+  </si>
+  <si>
+    <t>{"":""}</t>
   </si>
 </sst>
 </file>
@@ -2063,7 +2066,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
@@ -2096,9 +2099,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2384,7 +2384,7 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2432,8 +2432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A501"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="A106" sqref="A106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4959,9 +4959,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5083,7 +5081,7 @@
   <dimension ref="A1:A26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5357,7 +5355,7 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5367,22 +5365,22 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>84</v>
+        <v>648</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15">
-        <v>50016305</v>
+      <c r="A2" s="3" t="s">
+        <v>649</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>162</v>
+        <v>649</v>
       </c>
     </row>
   </sheetData>
@@ -5395,7 +5393,7 @@
   <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A9"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5554,7 +5552,7 @@
   <dimension ref="A1:A14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5815,9 +5813,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>